<commit_message>
documentation %26 message class
</commit_message>
<xml_diff>
--- a/src/zxxt_01_excel.xlsx.w3mi.data.xlsx
+++ b/src/zxxt_01_excel.xlsx.w3mi.data.xlsx
@@ -63,9 +63,6 @@
     <t>Just string</t>
   </si>
   <si>
-    <t>{R-STRING}</t>
-  </si>
-  <si>
     <t>Integer</t>
   </si>
   <si>
@@ -88,6 +85,9 @@
       </rPr>
       <t>{R-BOTTOM}</t>
     </r>
+  </si>
+  <si>
+    <t>{R-TEXT}</t>
   </si>
 </sst>
 </file>
@@ -554,9 +554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FAE5BAA-5943-423A-91C9-46DCD0649A5F}">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -583,15 +581,15 @@
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="6" t="s">
         <v>5</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="2:3" x14ac:dyDescent="0.25">
@@ -599,7 +597,7 @@
     </row>
     <row r="8" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>